<commit_message>
Created a new class EpsilonSort as an experiment to do sorted filtering on theta. Works a bit. Not sure if logic is wrong or if need more categories or it is just plain broken.
</commit_message>
<xml_diff>
--- a/results/ExploreAngles/angles.xlsx
+++ b/results/ExploreAngles/angles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/repos/github/angles/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/repos/github/angles/results/ExploreAngles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03DC9C5E-0A72-7948-A888-E7213BBFCEF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAA501C-8B73-D747-B7AB-338B6F5A64D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="4300" windowWidth="27640" windowHeight="16940" xr2:uid="{B9718DA1-5B9C-6A4D-81D1-0EFA79FA0301}"/>
+    <workbookView xWindow="40" yWindow="600" windowWidth="27640" windowHeight="16940" xr2:uid="{B9718DA1-5B9C-6A4D-81D1-0EFA79FA0301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Euc10: Summary for threshold = 0.23 n = 1000</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>d q soln</t>
+  </si>
+  <si>
+    <t>radians</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -207,7 +210,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -523,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4F73AD-1A81-C14D-B510-FA53C109919E}">
-  <dimension ref="A2:N38"/>
+  <dimension ref="A2:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +540,7 @@
     <col min="14" max="14" width="12" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J2" s="3" t="s">
         <v>36</v>
       </c>
@@ -553,8 +556,14 @@
       <c r="N2" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
         <v>31</v>
       </c>
@@ -576,8 +585,14 @@
       <c r="N3" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +618,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -628,8 +643,14 @@
       <c r="N5">
         <v>12.27</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <v>1.3171999999999999</v>
+      </c>
+      <c r="Q5">
+        <v>0.21415190000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -655,7 +676,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -681,7 +702,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -707,32 +728,32 @@
         <v>6.81</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -834,5 +855,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>